<commit_message>
Finish data collection for 2028 roster, fix errors in 2027 roster
</commit_message>
<xml_diff>
--- a/data/datasets/2027_team.xlsx
+++ b/data/datasets/2027_team.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28227"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28324"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\cdpet\Documents\Post School Coursework\data_projects\cfb-analysis\data\csv\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\cdpet\Documents\Post School Coursework\data_projects\cfb-analysis\data\datasets\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FD92A627-8A84-469A-BFA5-0BCB4C13E2FF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BFD93BC3-72AD-4F54-9506-D50407EF2880}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12720" xr2:uid="{9902822A-833C-4F31-A1F2-E8A6A5C2541E}"/>
   </bookViews>
@@ -141,9 +141,6 @@
     <t>Taylor</t>
   </si>
   <si>
-    <t>Linkcoln</t>
-  </si>
-  <si>
     <t>Vernon</t>
   </si>
   <si>
@@ -733,6 +730,9 @@
   </si>
   <si>
     <t>dev_trait</t>
+  </si>
+  <si>
+    <t>Lincoln</t>
   </si>
 </sst>
 </file>
@@ -1086,8 +1086,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DFAB4897-4CD3-4536-A31D-6A55B5AF8EA0}">
   <dimension ref="A1:J86"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="G84" sqref="G84"/>
+    <sheetView tabSelected="1" topLeftCell="A4" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="B20" sqref="B20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1105,34 +1105,34 @@
   <sheetData>
     <row r="1" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
+        <v>59</v>
+      </c>
+      <c r="B1" t="s">
         <v>60</v>
       </c>
-      <c r="B1" t="s">
+      <c r="C1" t="s">
+        <v>201</v>
+      </c>
+      <c r="D1" t="s">
+        <v>202</v>
+      </c>
+      <c r="E1" t="s">
         <v>61</v>
       </c>
-      <c r="C1" t="s">
-        <v>202</v>
-      </c>
-      <c r="D1" t="s">
-        <v>203</v>
-      </c>
-      <c r="E1" t="s">
+      <c r="F1" t="s">
         <v>62</v>
       </c>
-      <c r="F1" t="s">
+      <c r="G1" t="s">
         <v>63</v>
       </c>
-      <c r="G1" t="s">
-        <v>64</v>
-      </c>
       <c r="H1" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="I1" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="J1" t="s">
-        <v>235</v>
+        <v>234</v>
       </c>
     </row>
     <row r="2" spans="1:10" x14ac:dyDescent="0.3">
@@ -1143,7 +1143,7 @@
         <v>2</v>
       </c>
       <c r="C2" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
       <c r="D2" t="b">
         <v>1</v>
@@ -1158,13 +1158,13 @@
         <v>0</v>
       </c>
       <c r="H2" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="I2" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
       <c r="J2" t="s">
-        <v>231</v>
+        <v>230</v>
       </c>
     </row>
     <row r="3" spans="1:10" x14ac:dyDescent="0.3">
@@ -1175,7 +1175,7 @@
         <v>4</v>
       </c>
       <c r="C3" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
       <c r="D3" t="b">
         <v>0</v>
@@ -1190,13 +1190,13 @@
         <v>0</v>
       </c>
       <c r="H3" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="I3" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
       <c r="J3" t="s">
-        <v>232</v>
+        <v>231</v>
       </c>
     </row>
     <row r="4" spans="1:10" x14ac:dyDescent="0.3">
@@ -1207,7 +1207,7 @@
         <v>6</v>
       </c>
       <c r="C4" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
       <c r="D4" t="b">
         <v>0</v>
@@ -1222,13 +1222,13 @@
         <v>0</v>
       </c>
       <c r="H4" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="I4" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
       <c r="J4" t="s">
-        <v>231</v>
+        <v>230</v>
       </c>
     </row>
     <row r="5" spans="1:10" x14ac:dyDescent="0.3">
@@ -1239,7 +1239,7 @@
         <v>8</v>
       </c>
       <c r="C5" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
       <c r="D5" t="b">
         <v>0</v>
@@ -1254,13 +1254,13 @@
         <v>0</v>
       </c>
       <c r="H5" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="I5" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
       <c r="J5" t="s">
-        <v>231</v>
+        <v>230</v>
       </c>
     </row>
     <row r="6" spans="1:10" x14ac:dyDescent="0.3">
@@ -1271,7 +1271,7 @@
         <v>10</v>
       </c>
       <c r="C6" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
       <c r="D6" t="b">
         <v>0</v>
@@ -1280,19 +1280,19 @@
         <v>11</v>
       </c>
       <c r="F6" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="G6" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="H6" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="I6" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
       <c r="J6" t="s">
-        <v>231</v>
+        <v>230</v>
       </c>
     </row>
     <row r="7" spans="1:10" x14ac:dyDescent="0.3">
@@ -1303,7 +1303,7 @@
         <v>13</v>
       </c>
       <c r="C7" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
       <c r="D7" t="b">
         <v>1</v>
@@ -1312,19 +1312,19 @@
         <v>11</v>
       </c>
       <c r="F7" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="G7" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="H7" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="I7" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
       <c r="J7" t="s">
-        <v>231</v>
+        <v>230</v>
       </c>
     </row>
     <row r="8" spans="1:10" x14ac:dyDescent="0.3">
@@ -1335,7 +1335,7 @@
         <v>15</v>
       </c>
       <c r="C8" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
       <c r="D8" t="b">
         <v>0</v>
@@ -1344,19 +1344,19 @@
         <v>11</v>
       </c>
       <c r="F8" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="G8" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="H8" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="I8" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
       <c r="J8" t="s">
-        <v>231</v>
+        <v>230</v>
       </c>
     </row>
     <row r="9" spans="1:10" x14ac:dyDescent="0.3">
@@ -1367,7 +1367,7 @@
         <v>17</v>
       </c>
       <c r="C9" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
       <c r="D9" t="b">
         <v>1</v>
@@ -1376,19 +1376,19 @@
         <v>11</v>
       </c>
       <c r="F9" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="G9" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="H9" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="I9" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
       <c r="J9" t="s">
-        <v>233</v>
+        <v>232</v>
       </c>
     </row>
     <row r="10" spans="1:10" x14ac:dyDescent="0.3">
@@ -1399,7 +1399,7 @@
         <v>19</v>
       </c>
       <c r="C10" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
       <c r="D10" t="b">
         <v>1</v>
@@ -1408,19 +1408,19 @@
         <v>11</v>
       </c>
       <c r="F10" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="G10" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="H10" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="I10" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
       <c r="J10" t="s">
-        <v>231</v>
+        <v>230</v>
       </c>
     </row>
     <row r="11" spans="1:10" x14ac:dyDescent="0.3">
@@ -1431,7 +1431,7 @@
         <v>21</v>
       </c>
       <c r="C11" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
       <c r="D11" t="b">
         <v>0</v>
@@ -1440,19 +1440,19 @@
         <v>11</v>
       </c>
       <c r="F11" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="G11" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="H11" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="I11" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
       <c r="J11" t="s">
-        <v>232</v>
+        <v>231</v>
       </c>
     </row>
     <row r="12" spans="1:10" x14ac:dyDescent="0.3">
@@ -1463,7 +1463,7 @@
         <v>23</v>
       </c>
       <c r="C12" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
       <c r="D12" t="b">
         <v>0</v>
@@ -1472,19 +1472,19 @@
         <v>11</v>
       </c>
       <c r="F12" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="G12" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="H12" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="I12" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
       <c r="J12" t="s">
-        <v>231</v>
+        <v>230</v>
       </c>
     </row>
     <row r="13" spans="1:10" x14ac:dyDescent="0.3">
@@ -1495,7 +1495,7 @@
         <v>26</v>
       </c>
       <c r="C13" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
       <c r="D13" t="b">
         <v>1</v>
@@ -1507,16 +1507,16 @@
         <v>24</v>
       </c>
       <c r="G13" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="H13" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="I13" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
       <c r="J13" t="s">
-        <v>231</v>
+        <v>230</v>
       </c>
     </row>
     <row r="14" spans="1:10" x14ac:dyDescent="0.3">
@@ -1527,7 +1527,7 @@
         <v>28</v>
       </c>
       <c r="C14" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
       <c r="D14" t="b">
         <v>0</v>
@@ -1539,16 +1539,16 @@
         <v>24</v>
       </c>
       <c r="G14" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="H14" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="I14" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
       <c r="J14" t="s">
-        <v>233</v>
+        <v>232</v>
       </c>
     </row>
     <row r="15" spans="1:10" x14ac:dyDescent="0.3">
@@ -1559,7 +1559,7 @@
         <v>30</v>
       </c>
       <c r="C15" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
       <c r="D15" t="b">
         <v>0</v>
@@ -1571,16 +1571,16 @@
         <v>24</v>
       </c>
       <c r="G15" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="H15" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="I15" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
       <c r="J15" t="s">
-        <v>231</v>
+        <v>230</v>
       </c>
     </row>
     <row r="16" spans="1:10" x14ac:dyDescent="0.3">
@@ -1591,7 +1591,7 @@
         <v>32</v>
       </c>
       <c r="C16" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
       <c r="D16" t="b">
         <v>1</v>
@@ -1603,16 +1603,16 @@
         <v>24</v>
       </c>
       <c r="G16" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="H16" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="I16" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
       <c r="J16" t="s">
-        <v>231</v>
+        <v>230</v>
       </c>
     </row>
     <row r="17" spans="1:10" x14ac:dyDescent="0.3">
@@ -1623,7 +1623,7 @@
         <v>34</v>
       </c>
       <c r="C17" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
       <c r="D17" t="b">
         <v>1</v>
@@ -1635,16 +1635,16 @@
         <v>24</v>
       </c>
       <c r="G17" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="H17" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="I17" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
       <c r="J17" t="s">
-        <v>231</v>
+        <v>230</v>
       </c>
     </row>
     <row r="18" spans="1:10" x14ac:dyDescent="0.3">
@@ -1655,7 +1655,7 @@
         <v>36</v>
       </c>
       <c r="C18" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
       <c r="D18" t="b">
         <v>0</v>
@@ -1667,16 +1667,16 @@
         <v>24</v>
       </c>
       <c r="G18" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="H18" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="I18" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
       <c r="J18" t="s">
-        <v>232</v>
+        <v>231</v>
       </c>
     </row>
     <row r="19" spans="1:10" x14ac:dyDescent="0.3">
@@ -1684,10 +1684,10 @@
         <v>37</v>
       </c>
       <c r="B19" t="s">
-        <v>38</v>
+        <v>235</v>
       </c>
       <c r="C19" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
       <c r="D19" t="b">
         <v>0</v>
@@ -1699,27 +1699,27 @@
         <v>24</v>
       </c>
       <c r="G19" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="H19" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="I19" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
       <c r="J19" t="s">
-        <v>231</v>
+        <v>230</v>
       </c>
     </row>
     <row r="20" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A20" t="s">
+        <v>38</v>
+      </c>
+      <c r="B20" t="s">
         <v>39</v>
       </c>
-      <c r="B20" t="s">
-        <v>40</v>
-      </c>
       <c r="C20" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
       <c r="D20" t="b">
         <v>0</v>
@@ -1731,27 +1731,27 @@
         <v>24</v>
       </c>
       <c r="G20" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="H20" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="I20" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
       <c r="J20" t="s">
-        <v>231</v>
+        <v>230</v>
       </c>
     </row>
     <row r="21" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A21" t="s">
+        <v>40</v>
+      </c>
+      <c r="B21" t="s">
         <v>41</v>
       </c>
-      <c r="B21" t="s">
-        <v>42</v>
-      </c>
       <c r="C21" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
       <c r="D21" t="b">
         <v>0</v>
@@ -1763,2096 +1763,2096 @@
         <v>24</v>
       </c>
       <c r="G21" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="H21" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="I21" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
       <c r="J21" t="s">
-        <v>232</v>
+        <v>231</v>
       </c>
     </row>
     <row r="22" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A22" t="s">
+        <v>42</v>
+      </c>
+      <c r="B22" t="s">
         <v>43</v>
       </c>
-      <c r="B22" t="s">
-        <v>44</v>
-      </c>
       <c r="C22" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
       <c r="D22" t="b">
         <v>1</v>
       </c>
       <c r="E22" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="F22" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="G22" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="H22" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="I22" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="J22" t="s">
-        <v>231</v>
+        <v>230</v>
       </c>
     </row>
     <row r="23" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A23" t="s">
+        <v>44</v>
+      </c>
+      <c r="B23" t="s">
         <v>45</v>
       </c>
-      <c r="B23" t="s">
-        <v>46</v>
-      </c>
       <c r="C23" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
       <c r="D23" t="b">
         <v>1</v>
       </c>
       <c r="E23" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="F23" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="G23" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="H23" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="I23" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="J23" t="s">
-        <v>233</v>
+        <v>232</v>
       </c>
     </row>
     <row r="24" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A24" t="s">
+        <v>46</v>
+      </c>
+      <c r="B24" t="s">
         <v>47</v>
       </c>
-      <c r="B24" t="s">
-        <v>48</v>
-      </c>
       <c r="C24" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
       <c r="D24" t="b">
         <v>1</v>
       </c>
       <c r="E24" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="F24" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="G24" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="H24" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="I24" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
       <c r="J24" t="s">
-        <v>231</v>
+        <v>230</v>
       </c>
     </row>
     <row r="25" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A25" t="s">
+        <v>48</v>
+      </c>
+      <c r="B25" t="s">
         <v>49</v>
       </c>
-      <c r="B25" t="s">
+      <c r="C25" t="s">
+        <v>204</v>
+      </c>
+      <c r="D25" t="b">
+        <v>1</v>
+      </c>
+      <c r="E25" t="s">
         <v>50</v>
       </c>
-      <c r="C25" t="s">
-        <v>205</v>
-      </c>
-      <c r="D25" t="b">
-        <v>1</v>
-      </c>
-      <c r="E25" t="s">
-        <v>51</v>
-      </c>
       <c r="F25" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="G25" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="H25" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="I25" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
       <c r="J25" t="s">
-        <v>232</v>
+        <v>231</v>
       </c>
     </row>
     <row r="26" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A26" t="s">
+        <v>51</v>
+      </c>
+      <c r="B26" t="s">
         <v>52</v>
       </c>
-      <c r="B26" t="s">
+      <c r="C26" t="s">
+        <v>203</v>
+      </c>
+      <c r="D26" t="b">
+        <v>1</v>
+      </c>
+      <c r="E26" t="s">
+        <v>58</v>
+      </c>
+      <c r="F26" t="s">
         <v>53</v>
       </c>
-      <c r="C26" t="s">
-        <v>204</v>
-      </c>
-      <c r="D26" t="b">
-        <v>1</v>
-      </c>
-      <c r="E26" t="s">
-        <v>59</v>
-      </c>
-      <c r="F26" t="s">
-        <v>54</v>
-      </c>
       <c r="G26" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="H26" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="I26" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
       <c r="J26" t="s">
-        <v>231</v>
+        <v>230</v>
       </c>
     </row>
     <row r="27" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A27" t="s">
+        <v>54</v>
+      </c>
+      <c r="B27" t="s">
         <v>55</v>
       </c>
-      <c r="B27" t="s">
-        <v>56</v>
-      </c>
       <c r="C27" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
       <c r="D27" t="b">
         <v>1</v>
       </c>
       <c r="E27" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="F27" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="G27" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="H27" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="I27" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
       <c r="J27" t="s">
-        <v>232</v>
+        <v>231</v>
       </c>
     </row>
     <row r="28" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A28" t="s">
+        <v>56</v>
+      </c>
+      <c r="B28" t="s">
         <v>57</v>
       </c>
-      <c r="B28" t="s">
+      <c r="C28" t="s">
+        <v>204</v>
+      </c>
+      <c r="D28" t="b">
+        <v>0</v>
+      </c>
+      <c r="E28" t="s">
         <v>58</v>
       </c>
-      <c r="C28" t="s">
-        <v>205</v>
-      </c>
-      <c r="D28" t="b">
-        <v>0</v>
-      </c>
-      <c r="E28" t="s">
-        <v>59</v>
-      </c>
       <c r="F28" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="G28" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="H28" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="I28" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
       <c r="J28" t="s">
-        <v>231</v>
+        <v>230</v>
       </c>
     </row>
     <row r="29" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A29" t="s">
+        <v>67</v>
+      </c>
+      <c r="B29" t="s">
         <v>68</v>
       </c>
-      <c r="B29" t="s">
+      <c r="C29" t="s">
+        <v>206</v>
+      </c>
+      <c r="D29" t="b">
+        <v>1</v>
+      </c>
+      <c r="E29" t="s">
         <v>69</v>
       </c>
-      <c r="C29" t="s">
-        <v>207</v>
-      </c>
-      <c r="D29" t="b">
-        <v>1</v>
-      </c>
-      <c r="E29" t="s">
+      <c r="F29" t="s">
         <v>70</v>
       </c>
-      <c r="F29" t="s">
-        <v>71</v>
-      </c>
       <c r="G29" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="H29" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="I29" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
       <c r="J29" t="s">
-        <v>231</v>
+        <v>230</v>
       </c>
     </row>
     <row r="30" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A30" t="s">
+        <v>71</v>
+      </c>
+      <c r="B30" t="s">
         <v>72</v>
       </c>
-      <c r="B30" t="s">
-        <v>73</v>
-      </c>
       <c r="C30" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
       <c r="D30" t="b">
         <v>1</v>
       </c>
       <c r="E30" t="s">
+        <v>69</v>
+      </c>
+      <c r="F30" t="s">
         <v>70</v>
       </c>
-      <c r="F30" t="s">
-        <v>71</v>
-      </c>
       <c r="G30" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="H30" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="I30" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
       <c r="J30" t="s">
-        <v>232</v>
+        <v>231</v>
       </c>
     </row>
     <row r="31" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A31" t="s">
+        <v>73</v>
+      </c>
+      <c r="B31" t="s">
         <v>74</v>
       </c>
-      <c r="B31" t="s">
-        <v>75</v>
-      </c>
       <c r="C31" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
       <c r="D31" t="b">
         <v>0</v>
       </c>
       <c r="E31" t="s">
+        <v>69</v>
+      </c>
+      <c r="F31" t="s">
         <v>70</v>
       </c>
-      <c r="F31" t="s">
-        <v>71</v>
-      </c>
       <c r="G31" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="H31" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="I31" t="s">
-        <v>220</v>
+        <v>219</v>
       </c>
       <c r="J31" t="s">
-        <v>232</v>
+        <v>231</v>
       </c>
     </row>
     <row r="32" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A32" t="s">
+        <v>75</v>
+      </c>
+      <c r="B32" t="s">
         <v>76</v>
       </c>
-      <c r="B32" t="s">
+      <c r="C32" t="s">
+        <v>205</v>
+      </c>
+      <c r="D32" t="b">
+        <v>1</v>
+      </c>
+      <c r="E32" t="s">
         <v>77</v>
       </c>
-      <c r="C32" t="s">
-        <v>206</v>
-      </c>
-      <c r="D32" t="b">
-        <v>1</v>
-      </c>
-      <c r="E32" t="s">
-        <v>78</v>
-      </c>
       <c r="F32" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="G32" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="H32" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="I32" t="s">
-        <v>220</v>
+        <v>219</v>
       </c>
       <c r="J32" t="s">
-        <v>231</v>
+        <v>230</v>
       </c>
     </row>
     <row r="33" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A33" t="s">
+        <v>78</v>
+      </c>
+      <c r="B33" t="s">
         <v>79</v>
       </c>
-      <c r="B33" t="s">
-        <v>80</v>
-      </c>
       <c r="C33" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
       <c r="D33" t="b">
         <v>0</v>
       </c>
       <c r="E33" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="F33" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="G33" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="H33" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="I33" t="s">
-        <v>220</v>
+        <v>219</v>
       </c>
       <c r="J33" t="s">
-        <v>232</v>
+        <v>231</v>
       </c>
     </row>
     <row r="34" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A34" t="s">
+        <v>80</v>
+      </c>
+      <c r="B34" t="s">
         <v>81</v>
       </c>
-      <c r="B34" t="s">
-        <v>82</v>
-      </c>
       <c r="C34" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
       <c r="D34" t="b">
         <v>1</v>
       </c>
       <c r="E34" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="F34" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="G34" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="H34" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="I34" t="s">
-        <v>220</v>
+        <v>219</v>
       </c>
       <c r="J34" t="s">
-        <v>232</v>
+        <v>231</v>
       </c>
     </row>
     <row r="35" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A35" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="B35" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="C35" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
       <c r="D35" t="b">
         <v>1</v>
       </c>
       <c r="E35" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="F35" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="G35" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="H35" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="I35" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
       <c r="J35" t="s">
-        <v>231</v>
+        <v>230</v>
       </c>
     </row>
     <row r="36" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A36" t="s">
+        <v>83</v>
+      </c>
+      <c r="B36" t="s">
         <v>84</v>
       </c>
-      <c r="B36" t="s">
-        <v>85</v>
-      </c>
       <c r="C36" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
       <c r="D36" t="b">
         <v>1</v>
       </c>
       <c r="E36" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="F36" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="G36" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="H36" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="I36" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
       <c r="J36" t="s">
-        <v>234</v>
+        <v>233</v>
       </c>
     </row>
     <row r="37" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A37" t="s">
+        <v>85</v>
+      </c>
+      <c r="B37" t="s">
+        <v>72</v>
+      </c>
+      <c r="C37" t="s">
+        <v>204</v>
+      </c>
+      <c r="D37" t="b">
+        <v>0</v>
+      </c>
+      <c r="E37" t="s">
         <v>86</v>
       </c>
-      <c r="B37" t="s">
-        <v>73</v>
-      </c>
-      <c r="C37" t="s">
-        <v>205</v>
-      </c>
-      <c r="D37" t="b">
-        <v>0</v>
-      </c>
-      <c r="E37" t="s">
-        <v>87</v>
-      </c>
       <c r="F37" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="G37" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="H37" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="I37" t="s">
-        <v>220</v>
+        <v>219</v>
       </c>
       <c r="J37" t="s">
-        <v>232</v>
+        <v>231</v>
       </c>
     </row>
     <row r="38" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A38" t="s">
+        <v>87</v>
+      </c>
+      <c r="B38" t="s">
         <v>88</v>
       </c>
-      <c r="B38" t="s">
-        <v>89</v>
-      </c>
       <c r="C38" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
       <c r="D38" t="b">
         <v>1</v>
       </c>
       <c r="E38" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="F38" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="G38" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="H38" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="I38" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
       <c r="J38" t="s">
-        <v>232</v>
+        <v>231</v>
       </c>
     </row>
     <row r="39" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A39" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="B39" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="C39" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
       <c r="D39" t="b">
         <v>1</v>
       </c>
       <c r="E39" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="F39" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="G39" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="H39" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="I39" t="s">
-        <v>220</v>
+        <v>219</v>
       </c>
       <c r="J39" t="s">
-        <v>233</v>
+        <v>232</v>
       </c>
     </row>
     <row r="40" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A40" t="s">
+        <v>90</v>
+      </c>
+      <c r="B40" t="s">
         <v>91</v>
       </c>
-      <c r="B40" t="s">
+      <c r="C40" t="s">
+        <v>204</v>
+      </c>
+      <c r="D40" t="b">
+        <v>0</v>
+      </c>
+      <c r="E40" t="s">
         <v>92</v>
       </c>
-      <c r="C40" t="s">
-        <v>205</v>
-      </c>
-      <c r="D40" t="b">
-        <v>0</v>
-      </c>
-      <c r="E40" t="s">
-        <v>93</v>
-      </c>
       <c r="F40" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="G40" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="H40" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="I40" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
       <c r="J40" t="s">
-        <v>234</v>
+        <v>233</v>
       </c>
     </row>
     <row r="41" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A41" t="s">
+        <v>93</v>
+      </c>
+      <c r="B41" t="s">
         <v>94</v>
       </c>
-      <c r="B41" t="s">
-        <v>95</v>
-      </c>
       <c r="C41" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
       <c r="D41" t="b">
         <v>0</v>
       </c>
       <c r="E41" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="F41" t="s">
+        <v>104</v>
+      </c>
+      <c r="G41" t="s">
         <v>105</v>
       </c>
-      <c r="G41" t="s">
-        <v>106</v>
-      </c>
       <c r="H41" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="I41" t="s">
-        <v>221</v>
+        <v>220</v>
       </c>
       <c r="J41" t="s">
-        <v>233</v>
+        <v>232</v>
       </c>
     </row>
     <row r="42" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A42" t="s">
+        <v>95</v>
+      </c>
+      <c r="B42" t="s">
         <v>96</v>
       </c>
-      <c r="B42" t="s">
-        <v>97</v>
-      </c>
       <c r="C42" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
       <c r="D42" t="b">
         <v>0</v>
       </c>
       <c r="E42" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="F42" t="s">
+        <v>104</v>
+      </c>
+      <c r="G42" t="s">
         <v>105</v>
       </c>
-      <c r="G42" t="s">
-        <v>106</v>
-      </c>
       <c r="H42" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="I42" t="s">
-        <v>221</v>
+        <v>220</v>
       </c>
       <c r="J42" t="s">
-        <v>234</v>
+        <v>233</v>
       </c>
     </row>
     <row r="43" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A43" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="B43" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="C43" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
       <c r="D43" t="b">
         <v>1</v>
       </c>
       <c r="E43" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="F43" t="s">
+        <v>104</v>
+      </c>
+      <c r="G43" t="s">
         <v>105</v>
       </c>
-      <c r="G43" t="s">
-        <v>106</v>
-      </c>
       <c r="H43" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="I43" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
       <c r="J43" t="s">
-        <v>231</v>
+        <v>230</v>
       </c>
     </row>
     <row r="44" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A44" t="s">
+        <v>98</v>
+      </c>
+      <c r="B44" t="s">
         <v>99</v>
       </c>
-      <c r="B44" t="s">
+      <c r="C44" t="s">
+        <v>204</v>
+      </c>
+      <c r="D44" t="b">
+        <v>0</v>
+      </c>
+      <c r="E44" t="s">
         <v>100</v>
       </c>
-      <c r="C44" t="s">
-        <v>205</v>
-      </c>
-      <c r="D44" t="b">
-        <v>0</v>
-      </c>
-      <c r="E44" t="s">
-        <v>101</v>
-      </c>
       <c r="F44" t="s">
+        <v>104</v>
+      </c>
+      <c r="G44" t="s">
         <v>105</v>
       </c>
-      <c r="G44" t="s">
-        <v>106</v>
-      </c>
       <c r="H44" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="I44" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
       <c r="J44" t="s">
-        <v>232</v>
+        <v>231</v>
       </c>
     </row>
     <row r="45" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A45" t="s">
+        <v>106</v>
+      </c>
+      <c r="B45" t="s">
         <v>107</v>
       </c>
-      <c r="B45" t="s">
-        <v>108</v>
-      </c>
       <c r="C45" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
       <c r="D45" t="b">
         <v>0</v>
       </c>
       <c r="E45" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="F45" t="s">
+        <v>104</v>
+      </c>
+      <c r="G45" t="s">
         <v>105</v>
       </c>
-      <c r="G45" t="s">
-        <v>106</v>
-      </c>
       <c r="H45" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="I45" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
       <c r="J45" t="s">
-        <v>231</v>
+        <v>230</v>
       </c>
     </row>
     <row r="46" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A46" t="s">
+        <v>108</v>
+      </c>
+      <c r="B46" t="s">
         <v>109</v>
       </c>
-      <c r="B46" t="s">
-        <v>110</v>
-      </c>
       <c r="C46" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
       <c r="D46" t="b">
         <v>1</v>
       </c>
       <c r="E46" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="F46" t="s">
+        <v>104</v>
+      </c>
+      <c r="G46" t="s">
         <v>105</v>
       </c>
-      <c r="G46" t="s">
-        <v>106</v>
-      </c>
       <c r="H46" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="I46" t="s">
-        <v>221</v>
+        <v>220</v>
       </c>
       <c r="J46" t="s">
-        <v>231</v>
+        <v>230</v>
       </c>
     </row>
     <row r="47" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A47" t="s">
+        <v>110</v>
+      </c>
+      <c r="B47" t="s">
         <v>111</v>
       </c>
-      <c r="B47" t="s">
-        <v>112</v>
-      </c>
       <c r="C47" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
       <c r="D47" t="b">
         <v>1</v>
       </c>
       <c r="E47" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="F47" t="s">
+        <v>104</v>
+      </c>
+      <c r="G47" t="s">
         <v>105</v>
       </c>
-      <c r="G47" t="s">
-        <v>106</v>
-      </c>
       <c r="H47" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="I47" t="s">
-        <v>221</v>
+        <v>220</v>
       </c>
       <c r="J47" t="s">
-        <v>231</v>
+        <v>230</v>
       </c>
     </row>
     <row r="48" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A48" t="s">
+        <v>112</v>
+      </c>
+      <c r="B48" t="s">
         <v>113</v>
       </c>
-      <c r="B48" t="s">
-        <v>114</v>
-      </c>
       <c r="C48" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
       <c r="D48" t="b">
         <v>1</v>
       </c>
       <c r="E48" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="F48" t="s">
+        <v>104</v>
+      </c>
+      <c r="G48" t="s">
         <v>105</v>
       </c>
-      <c r="G48" t="s">
-        <v>106</v>
-      </c>
       <c r="H48" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="I48" t="s">
-        <v>221</v>
+        <v>220</v>
       </c>
       <c r="J48" t="s">
-        <v>233</v>
+        <v>232</v>
       </c>
     </row>
     <row r="49" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A49" t="s">
+        <v>114</v>
+      </c>
+      <c r="B49" t="s">
         <v>115</v>
       </c>
-      <c r="B49" t="s">
+      <c r="C49" t="s">
+        <v>204</v>
+      </c>
+      <c r="D49" t="b">
+        <v>0</v>
+      </c>
+      <c r="E49" t="s">
         <v>116</v>
       </c>
-      <c r="C49" t="s">
-        <v>205</v>
-      </c>
-      <c r="D49" t="b">
-        <v>0</v>
-      </c>
-      <c r="E49" t="s">
-        <v>117</v>
-      </c>
       <c r="F49" t="s">
+        <v>104</v>
+      </c>
+      <c r="G49" t="s">
         <v>105</v>
       </c>
-      <c r="G49" t="s">
-        <v>106</v>
-      </c>
       <c r="H49" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="I49" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
       <c r="J49" t="s">
-        <v>234</v>
+        <v>233</v>
       </c>
     </row>
     <row r="50" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A50" t="s">
+        <v>117</v>
+      </c>
+      <c r="B50" t="s">
         <v>118</v>
       </c>
-      <c r="B50" t="s">
-        <v>119</v>
-      </c>
       <c r="C50" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
       <c r="D50" t="b">
         <v>1</v>
       </c>
       <c r="E50" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="F50" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="G50" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="H50" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="I50" t="s">
-        <v>221</v>
+        <v>220</v>
       </c>
       <c r="J50" t="s">
-        <v>231</v>
+        <v>230</v>
       </c>
     </row>
     <row r="51" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A51" t="s">
+        <v>119</v>
+      </c>
+      <c r="B51" t="s">
         <v>120</v>
       </c>
-      <c r="B51" t="s">
-        <v>121</v>
-      </c>
       <c r="C51" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
       <c r="D51" t="b">
         <v>0</v>
       </c>
       <c r="E51" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="F51" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="G51" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="H51" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="I51" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
       <c r="J51" t="s">
-        <v>231</v>
+        <v>230</v>
       </c>
     </row>
     <row r="52" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A52" t="s">
+        <v>121</v>
+      </c>
+      <c r="B52" t="s">
         <v>122</v>
       </c>
-      <c r="B52" t="s">
-        <v>123</v>
-      </c>
       <c r="C52" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
       <c r="D52" t="b">
         <v>0</v>
       </c>
       <c r="E52" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="F52" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="G52" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="H52" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="I52" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
       <c r="J52" t="s">
-        <v>231</v>
+        <v>230</v>
       </c>
     </row>
     <row r="53" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A53" t="s">
+        <v>123</v>
+      </c>
+      <c r="B53" t="s">
         <v>124</v>
       </c>
-      <c r="B53" t="s">
-        <v>125</v>
-      </c>
       <c r="C53" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
       <c r="D53" t="b">
         <v>1</v>
       </c>
       <c r="E53" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="F53" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="G53" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="H53" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="I53" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
       <c r="J53" t="s">
-        <v>231</v>
+        <v>230</v>
       </c>
     </row>
     <row r="54" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A54" t="s">
+        <v>125</v>
+      </c>
+      <c r="B54" t="s">
         <v>126</v>
       </c>
-      <c r="B54" t="s">
-        <v>127</v>
-      </c>
       <c r="C54" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
       <c r="D54" t="b">
         <v>0</v>
       </c>
       <c r="E54" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="F54" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="G54" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="H54" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="I54" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
       <c r="J54" t="s">
-        <v>231</v>
+        <v>230</v>
       </c>
     </row>
     <row r="55" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A55" t="s">
+        <v>127</v>
+      </c>
+      <c r="B55" t="s">
         <v>128</v>
       </c>
-      <c r="B55" t="s">
+      <c r="C55" t="s">
+        <v>204</v>
+      </c>
+      <c r="D55" t="b">
+        <v>0</v>
+      </c>
+      <c r="E55" t="s">
         <v>129</v>
       </c>
-      <c r="C55" t="s">
-        <v>205</v>
-      </c>
-      <c r="D55" t="b">
-        <v>0</v>
-      </c>
-      <c r="E55" t="s">
-        <v>130</v>
-      </c>
       <c r="F55" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="G55" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="H55" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="I55" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
       <c r="J55" t="s">
-        <v>231</v>
+        <v>230</v>
       </c>
     </row>
     <row r="56" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A56" t="s">
+        <v>130</v>
+      </c>
+      <c r="B56" t="s">
         <v>131</v>
       </c>
-      <c r="B56" t="s">
-        <v>132</v>
-      </c>
       <c r="C56" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
       <c r="D56" t="b">
         <v>0</v>
       </c>
       <c r="E56" t="s">
+        <v>138</v>
+      </c>
+      <c r="F56" t="s">
         <v>139</v>
       </c>
-      <c r="F56" t="s">
+      <c r="G56" t="s">
         <v>140</v>
       </c>
-      <c r="G56" t="s">
-        <v>141</v>
-      </c>
       <c r="H56" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="I56" t="s">
-        <v>221</v>
+        <v>220</v>
       </c>
       <c r="J56" t="s">
-        <v>232</v>
+        <v>231</v>
       </c>
     </row>
     <row r="57" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A57" t="s">
+        <v>132</v>
+      </c>
+      <c r="B57" t="s">
         <v>133</v>
       </c>
-      <c r="B57" t="s">
-        <v>134</v>
-      </c>
       <c r="C57" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
       <c r="D57" t="b">
         <v>1</v>
       </c>
       <c r="E57" t="s">
+        <v>138</v>
+      </c>
+      <c r="F57" t="s">
         <v>139</v>
       </c>
-      <c r="F57" t="s">
+      <c r="G57" t="s">
         <v>140</v>
       </c>
-      <c r="G57" t="s">
-        <v>141</v>
-      </c>
       <c r="H57" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="I57" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
       <c r="J57" t="s">
-        <v>231</v>
+        <v>230</v>
       </c>
     </row>
     <row r="58" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A58" t="s">
+        <v>134</v>
+      </c>
+      <c r="B58" t="s">
         <v>135</v>
       </c>
-      <c r="B58" t="s">
-        <v>136</v>
-      </c>
       <c r="C58" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
       <c r="D58" t="b">
         <v>0</v>
       </c>
       <c r="E58" t="s">
+        <v>138</v>
+      </c>
+      <c r="F58" t="s">
         <v>139</v>
       </c>
-      <c r="F58" t="s">
+      <c r="G58" t="s">
         <v>140</v>
       </c>
-      <c r="G58" t="s">
-        <v>141</v>
-      </c>
       <c r="H58" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="I58" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
       <c r="J58" t="s">
-        <v>231</v>
+        <v>230</v>
       </c>
     </row>
     <row r="59" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A59" t="s">
+        <v>136</v>
+      </c>
+      <c r="B59" t="s">
         <v>137</v>
       </c>
-      <c r="B59" t="s">
+      <c r="C59" t="s">
+        <v>204</v>
+      </c>
+      <c r="D59" t="b">
+        <v>0</v>
+      </c>
+      <c r="E59" t="s">
         <v>138</v>
       </c>
-      <c r="C59" t="s">
-        <v>205</v>
-      </c>
-      <c r="D59" t="b">
-        <v>0</v>
-      </c>
-      <c r="E59" t="s">
+      <c r="F59" t="s">
         <v>139</v>
       </c>
-      <c r="F59" t="s">
+      <c r="G59" t="s">
         <v>140</v>
       </c>
-      <c r="G59" t="s">
-        <v>141</v>
-      </c>
       <c r="H59" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="I59" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
       <c r="J59" t="s">
-        <v>233</v>
+        <v>232</v>
       </c>
     </row>
     <row r="60" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A60" t="s">
+        <v>141</v>
+      </c>
+      <c r="B60" t="s">
         <v>142</v>
       </c>
-      <c r="B60" t="s">
-        <v>143</v>
-      </c>
       <c r="C60" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
       <c r="D60" t="b">
         <v>1</v>
       </c>
       <c r="E60" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="F60" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="G60" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="H60" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="I60" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
       <c r="J60" t="s">
-        <v>231</v>
+        <v>230</v>
       </c>
     </row>
     <row r="61" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A61" t="s">
+        <v>143</v>
+      </c>
+      <c r="B61" t="s">
         <v>144</v>
       </c>
-      <c r="B61" t="s">
-        <v>145</v>
-      </c>
       <c r="C61" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
       <c r="D61" t="b">
         <v>1</v>
       </c>
       <c r="E61" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="F61" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="G61" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="H61" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="I61" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
       <c r="J61" t="s">
-        <v>231</v>
+        <v>230</v>
       </c>
     </row>
     <row r="62" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A62" t="s">
+        <v>145</v>
+      </c>
+      <c r="B62" t="s">
         <v>146</v>
       </c>
-      <c r="B62" t="s">
+      <c r="C62" t="s">
+        <v>204</v>
+      </c>
+      <c r="D62" t="b">
+        <v>0</v>
+      </c>
+      <c r="E62" t="s">
         <v>147</v>
       </c>
-      <c r="C62" t="s">
-        <v>205</v>
-      </c>
-      <c r="D62" t="b">
-        <v>0</v>
-      </c>
-      <c r="E62" t="s">
-        <v>148</v>
-      </c>
       <c r="F62" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="G62" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="H62" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="I62" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
       <c r="J62" t="s">
-        <v>233</v>
+        <v>232</v>
       </c>
     </row>
     <row r="63" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A63" t="s">
+        <v>148</v>
+      </c>
+      <c r="B63" t="s">
         <v>149</v>
       </c>
-      <c r="B63" t="s">
-        <v>150</v>
-      </c>
       <c r="C63" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
       <c r="D63" t="b">
         <v>1</v>
       </c>
       <c r="E63" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="F63" t="s">
+        <v>139</v>
+      </c>
+      <c r="G63" t="s">
         <v>140</v>
       </c>
-      <c r="G63" t="s">
-        <v>141</v>
-      </c>
       <c r="H63" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="I63" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
       <c r="J63" t="s">
-        <v>231</v>
+        <v>230</v>
       </c>
     </row>
     <row r="64" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A64" t="s">
+        <v>150</v>
+      </c>
+      <c r="B64" t="s">
         <v>151</v>
       </c>
-      <c r="B64" t="s">
-        <v>152</v>
-      </c>
       <c r="C64" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
       <c r="D64" t="b">
         <v>0</v>
       </c>
       <c r="E64" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="F64" t="s">
+        <v>139</v>
+      </c>
+      <c r="G64" t="s">
         <v>140</v>
       </c>
-      <c r="G64" t="s">
-        <v>141</v>
-      </c>
       <c r="H64" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="I64" t="s">
-        <v>221</v>
+        <v>220</v>
       </c>
       <c r="J64" t="s">
-        <v>232</v>
+        <v>231</v>
       </c>
     </row>
     <row r="65" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A65" t="s">
+        <v>152</v>
+      </c>
+      <c r="B65" t="s">
         <v>153</v>
       </c>
-      <c r="B65" t="s">
-        <v>154</v>
-      </c>
       <c r="C65" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
       <c r="D65" t="b">
         <v>1</v>
       </c>
       <c r="E65" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="F65" t="s">
+        <v>139</v>
+      </c>
+      <c r="G65" t="s">
         <v>140</v>
       </c>
-      <c r="G65" t="s">
-        <v>141</v>
-      </c>
       <c r="H65" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="I65" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
       <c r="J65" t="s">
-        <v>231</v>
+        <v>230</v>
       </c>
     </row>
     <row r="66" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A66" t="s">
+        <v>154</v>
+      </c>
+      <c r="B66" t="s">
         <v>155</v>
       </c>
-      <c r="B66" t="s">
+      <c r="C66" t="s">
+        <v>204</v>
+      </c>
+      <c r="D66" t="b">
+        <v>1</v>
+      </c>
+      <c r="E66" t="s">
         <v>156</v>
       </c>
-      <c r="C66" t="s">
-        <v>205</v>
-      </c>
-      <c r="D66" t="b">
-        <v>1</v>
-      </c>
-      <c r="E66" t="s">
-        <v>157</v>
-      </c>
       <c r="F66" t="s">
+        <v>139</v>
+      </c>
+      <c r="G66" t="s">
         <v>140</v>
       </c>
-      <c r="G66" t="s">
-        <v>141</v>
-      </c>
       <c r="H66" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="I66" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
       <c r="J66" t="s">
-        <v>232</v>
+        <v>231</v>
       </c>
     </row>
     <row r="67" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A67" t="s">
+        <v>157</v>
+      </c>
+      <c r="B67" t="s">
         <v>158</v>
       </c>
-      <c r="B67" t="s">
-        <v>159</v>
-      </c>
       <c r="C67" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
       <c r="D67" t="b">
         <v>1</v>
       </c>
       <c r="E67" t="s">
+        <v>172</v>
+      </c>
+      <c r="F67" t="s">
+        <v>172</v>
+      </c>
+      <c r="G67" t="s">
         <v>173</v>
       </c>
-      <c r="F67" t="s">
-        <v>173</v>
-      </c>
-      <c r="G67" t="s">
-        <v>174</v>
-      </c>
       <c r="H67" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="I67" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
       <c r="J67" t="s">
-        <v>233</v>
+        <v>232</v>
       </c>
     </row>
     <row r="68" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A68" t="s">
+        <v>159</v>
+      </c>
+      <c r="B68" t="s">
         <v>160</v>
       </c>
-      <c r="B68" t="s">
-        <v>161</v>
-      </c>
       <c r="C68" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
       <c r="D68" t="b">
         <v>1</v>
       </c>
       <c r="E68" t="s">
+        <v>172</v>
+      </c>
+      <c r="F68" t="s">
+        <v>172</v>
+      </c>
+      <c r="G68" t="s">
         <v>173</v>
       </c>
-      <c r="F68" t="s">
-        <v>173</v>
-      </c>
-      <c r="G68" t="s">
-        <v>174</v>
-      </c>
       <c r="H68" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="I68" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
       <c r="J68" t="s">
-        <v>231</v>
+        <v>230</v>
       </c>
     </row>
     <row r="69" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A69" t="s">
+        <v>161</v>
+      </c>
+      <c r="B69" t="s">
         <v>162</v>
       </c>
-      <c r="B69" t="s">
-        <v>163</v>
-      </c>
       <c r="C69" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
       <c r="D69" t="b">
         <v>1</v>
       </c>
       <c r="E69" t="s">
+        <v>172</v>
+      </c>
+      <c r="F69" t="s">
+        <v>172</v>
+      </c>
+      <c r="G69" t="s">
         <v>173</v>
       </c>
-      <c r="F69" t="s">
-        <v>173</v>
-      </c>
-      <c r="G69" t="s">
-        <v>174</v>
-      </c>
       <c r="H69" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="I69" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
       <c r="J69" t="s">
-        <v>233</v>
+        <v>232</v>
       </c>
     </row>
     <row r="70" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A70" t="s">
+        <v>163</v>
+      </c>
+      <c r="B70" t="s">
         <v>164</v>
       </c>
-      <c r="B70" t="s">
-        <v>165</v>
-      </c>
       <c r="C70" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
       <c r="D70" t="b">
         <v>0</v>
       </c>
       <c r="E70" t="s">
+        <v>172</v>
+      </c>
+      <c r="F70" t="s">
+        <v>172</v>
+      </c>
+      <c r="G70" t="s">
         <v>173</v>
       </c>
-      <c r="F70" t="s">
-        <v>173</v>
-      </c>
-      <c r="G70" t="s">
-        <v>174</v>
-      </c>
       <c r="H70" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="I70" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
       <c r="J70" t="s">
-        <v>231</v>
+        <v>230</v>
       </c>
     </row>
     <row r="71" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A71" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="B71" t="s">
         <v>30</v>
       </c>
       <c r="C71" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
       <c r="D71" t="b">
         <v>0</v>
       </c>
       <c r="E71" t="s">
+        <v>172</v>
+      </c>
+      <c r="F71" t="s">
+        <v>172</v>
+      </c>
+      <c r="G71" t="s">
         <v>173</v>
       </c>
-      <c r="F71" t="s">
-        <v>173</v>
-      </c>
-      <c r="G71" t="s">
-        <v>174</v>
-      </c>
       <c r="H71" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="I71" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
       <c r="J71" t="s">
-        <v>231</v>
+        <v>230</v>
       </c>
     </row>
     <row r="72" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A72" t="s">
+        <v>166</v>
+      </c>
+      <c r="B72" t="s">
         <v>167</v>
       </c>
-      <c r="B72" t="s">
-        <v>168</v>
-      </c>
       <c r="C72" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
       <c r="D72" t="b">
         <v>0</v>
       </c>
       <c r="E72" t="s">
+        <v>172</v>
+      </c>
+      <c r="F72" t="s">
+        <v>172</v>
+      </c>
+      <c r="G72" t="s">
         <v>173</v>
       </c>
-      <c r="F72" t="s">
-        <v>173</v>
-      </c>
-      <c r="G72" t="s">
-        <v>174</v>
-      </c>
       <c r="H72" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="I72" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
       <c r="J72" t="s">
-        <v>232</v>
+        <v>231</v>
       </c>
     </row>
     <row r="73" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A73" t="s">
+        <v>168</v>
+      </c>
+      <c r="B73" t="s">
         <v>169</v>
       </c>
-      <c r="B73" t="s">
-        <v>170</v>
-      </c>
       <c r="C73" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
       <c r="D73" t="b">
         <v>0</v>
       </c>
       <c r="E73" t="s">
+        <v>172</v>
+      </c>
+      <c r="F73" t="s">
+        <v>172</v>
+      </c>
+      <c r="G73" t="s">
         <v>173</v>
       </c>
-      <c r="F73" t="s">
-        <v>173</v>
-      </c>
-      <c r="G73" t="s">
-        <v>174</v>
-      </c>
       <c r="H73" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="I73" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
       <c r="J73" t="s">
-        <v>233</v>
+        <v>232</v>
       </c>
     </row>
     <row r="74" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A74" t="s">
+        <v>170</v>
+      </c>
+      <c r="B74" t="s">
         <v>171</v>
       </c>
-      <c r="B74" t="s">
+      <c r="C74" t="s">
+        <v>204</v>
+      </c>
+      <c r="D74" t="b">
+        <v>0</v>
+      </c>
+      <c r="E74" t="s">
         <v>172</v>
       </c>
-      <c r="C74" t="s">
-        <v>205</v>
-      </c>
-      <c r="D74" t="b">
-        <v>0</v>
-      </c>
-      <c r="E74" t="s">
+      <c r="F74" t="s">
+        <v>172</v>
+      </c>
+      <c r="G74" t="s">
         <v>173</v>
       </c>
-      <c r="F74" t="s">
-        <v>173</v>
-      </c>
-      <c r="G74" t="s">
-        <v>174</v>
-      </c>
       <c r="H74" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="I74" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
       <c r="J74" t="s">
-        <v>233</v>
+        <v>232</v>
       </c>
     </row>
     <row r="75" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A75" t="s">
+        <v>174</v>
+      </c>
+      <c r="B75" t="s">
         <v>175</v>
       </c>
-      <c r="B75" t="s">
-        <v>176</v>
-      </c>
       <c r="C75" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
       <c r="D75" t="b">
         <v>1</v>
       </c>
       <c r="E75" t="s">
+        <v>183</v>
+      </c>
+      <c r="F75" t="s">
         <v>184</v>
       </c>
-      <c r="F75" t="s">
-        <v>185</v>
-      </c>
       <c r="G75" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="H75" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="I75" t="s">
-        <v>227</v>
+        <v>226</v>
       </c>
       <c r="J75" t="s">
-        <v>231</v>
+        <v>230</v>
       </c>
     </row>
     <row r="76" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A76" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
       <c r="B76" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="C76" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
       <c r="D76" t="b">
         <v>1</v>
       </c>
       <c r="E76" t="s">
+        <v>183</v>
+      </c>
+      <c r="F76" t="s">
         <v>184</v>
       </c>
-      <c r="F76" t="s">
-        <v>185</v>
-      </c>
       <c r="G76" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="H76" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="I76" t="s">
-        <v>227</v>
+        <v>226</v>
       </c>
       <c r="J76" t="s">
-        <v>233</v>
+        <v>232</v>
       </c>
     </row>
     <row r="77" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A77" t="s">
+        <v>177</v>
+      </c>
+      <c r="B77" t="s">
         <v>178</v>
       </c>
-      <c r="B77" t="s">
-        <v>179</v>
-      </c>
       <c r="C77" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
       <c r="D77" t="b">
         <v>0</v>
       </c>
       <c r="E77" t="s">
+        <v>183</v>
+      </c>
+      <c r="F77" t="s">
         <v>184</v>
       </c>
-      <c r="F77" t="s">
-        <v>185</v>
-      </c>
       <c r="G77" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="H77" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="I77" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
       <c r="J77" t="s">
-        <v>232</v>
+        <v>231</v>
       </c>
     </row>
     <row r="78" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A78" t="s">
+        <v>179</v>
+      </c>
+      <c r="B78" t="s">
         <v>180</v>
       </c>
-      <c r="B78" t="s">
-        <v>181</v>
-      </c>
       <c r="C78" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
       <c r="D78" t="b">
         <v>0</v>
       </c>
       <c r="E78" t="s">
+        <v>183</v>
+      </c>
+      <c r="F78" t="s">
         <v>184</v>
       </c>
-      <c r="F78" t="s">
-        <v>185</v>
-      </c>
       <c r="G78" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="H78" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="I78" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
       <c r="J78" t="s">
-        <v>231</v>
+        <v>230</v>
       </c>
     </row>
     <row r="79" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A79" t="s">
+        <v>181</v>
+      </c>
+      <c r="B79" t="s">
         <v>182</v>
       </c>
-      <c r="B79" t="s">
+      <c r="C79" t="s">
+        <v>204</v>
+      </c>
+      <c r="D79" t="b">
+        <v>0</v>
+      </c>
+      <c r="E79" t="s">
         <v>183</v>
       </c>
-      <c r="C79" t="s">
-        <v>205</v>
-      </c>
-      <c r="D79" t="b">
-        <v>0</v>
-      </c>
-      <c r="E79" t="s">
+      <c r="F79" t="s">
         <v>184</v>
       </c>
-      <c r="F79" t="s">
-        <v>185</v>
-      </c>
       <c r="G79" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="H79" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="I79" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
       <c r="J79" t="s">
-        <v>231</v>
+        <v>230</v>
       </c>
     </row>
     <row r="80" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A80" t="s">
+        <v>185</v>
+      </c>
+      <c r="B80" t="s">
         <v>186</v>
       </c>
-      <c r="B80" t="s">
-        <v>187</v>
-      </c>
       <c r="C80" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
       <c r="D80" t="b">
         <v>0</v>
       </c>
       <c r="E80" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
       <c r="F80" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
       <c r="G80" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="H80" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="I80" t="s">
-        <v>229</v>
+        <v>228</v>
       </c>
       <c r="J80" t="s">
-        <v>231</v>
+        <v>230</v>
       </c>
     </row>
     <row r="81" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A81" t="s">
+        <v>187</v>
+      </c>
+      <c r="B81" t="s">
         <v>188</v>
       </c>
-      <c r="B81" t="s">
-        <v>189</v>
-      </c>
       <c r="C81" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
       <c r="D81" t="b">
         <v>1</v>
       </c>
       <c r="E81" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
       <c r="F81" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
       <c r="G81" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="H81" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="I81" t="s">
-        <v>229</v>
+        <v>228</v>
       </c>
       <c r="J81" t="s">
-        <v>234</v>
+        <v>233</v>
       </c>
     </row>
     <row r="82" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A82" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="B82" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
       <c r="C82" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
       <c r="D82" t="b">
         <v>0</v>
       </c>
       <c r="E82" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
       <c r="F82" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
       <c r="G82" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="H82" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="I82" t="s">
-        <v>227</v>
+        <v>226</v>
       </c>
       <c r="J82" t="s">
-        <v>231</v>
+        <v>230</v>
       </c>
     </row>
     <row r="83" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A83" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
       <c r="B83" t="s">
+        <v>190</v>
+      </c>
+      <c r="C83" t="s">
+        <v>204</v>
+      </c>
+      <c r="D83" t="b">
+        <v>1</v>
+      </c>
+      <c r="E83" t="s">
         <v>191</v>
       </c>
-      <c r="C83" t="s">
-        <v>205</v>
-      </c>
-      <c r="D83" t="b">
-        <v>1</v>
-      </c>
-      <c r="E83" t="s">
-        <v>192</v>
-      </c>
       <c r="F83" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
       <c r="G83" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="H83" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="I83" t="s">
-        <v>227</v>
+        <v>226</v>
       </c>
       <c r="J83" t="s">
-        <v>231</v>
+        <v>230</v>
       </c>
     </row>
     <row r="84" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A84" t="s">
+        <v>192</v>
+      </c>
+      <c r="B84" t="s">
         <v>193</v>
       </c>
-      <c r="B84" t="s">
-        <v>194</v>
-      </c>
       <c r="C84" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
       <c r="D84" t="b">
         <v>1</v>
       </c>
       <c r="E84" t="s">
+        <v>195</v>
+      </c>
+      <c r="F84" t="s">
+        <v>195</v>
+      </c>
+      <c r="G84" t="s">
+        <v>195</v>
+      </c>
+      <c r="H84" t="s">
         <v>196</v>
       </c>
-      <c r="F84" t="s">
-        <v>196</v>
-      </c>
-      <c r="G84" t="s">
-        <v>196</v>
-      </c>
-      <c r="H84" t="s">
-        <v>197</v>
-      </c>
       <c r="I84" t="s">
-        <v>230</v>
+        <v>229</v>
       </c>
       <c r="J84" t="s">
-        <v>233</v>
+        <v>232</v>
       </c>
     </row>
     <row r="85" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A85" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="B85" t="s">
+        <v>194</v>
+      </c>
+      <c r="C85" t="s">
+        <v>204</v>
+      </c>
+      <c r="D85" t="b">
+        <v>1</v>
+      </c>
+      <c r="E85" t="s">
         <v>195</v>
       </c>
-      <c r="C85" t="s">
-        <v>205</v>
-      </c>
-      <c r="D85" t="b">
-        <v>1</v>
-      </c>
-      <c r="E85" t="s">
+      <c r="F85" t="s">
+        <v>195</v>
+      </c>
+      <c r="G85" t="s">
+        <v>195</v>
+      </c>
+      <c r="H85" t="s">
         <v>196</v>
       </c>
-      <c r="F85" t="s">
-        <v>196</v>
-      </c>
-      <c r="G85" t="s">
-        <v>196</v>
-      </c>
-      <c r="H85" t="s">
-        <v>197</v>
-      </c>
       <c r="I85" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
       <c r="J85" t="s">
-        <v>231</v>
+        <v>230</v>
       </c>
     </row>
     <row r="86" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A86" t="s">
+        <v>197</v>
+      </c>
+      <c r="B86" t="s">
         <v>198</v>
       </c>
-      <c r="B86" t="s">
+      <c r="C86" t="s">
+        <v>204</v>
+      </c>
+      <c r="D86" t="b">
+        <v>0</v>
+      </c>
+      <c r="E86" t="s">
         <v>199</v>
       </c>
-      <c r="C86" t="s">
-        <v>205</v>
-      </c>
-      <c r="D86" t="b">
-        <v>0</v>
-      </c>
-      <c r="E86" t="s">
-        <v>200</v>
-      </c>
       <c r="F86" t="s">
+        <v>195</v>
+      </c>
+      <c r="G86" t="s">
+        <v>195</v>
+      </c>
+      <c r="H86" t="s">
         <v>196</v>
       </c>
-      <c r="G86" t="s">
-        <v>196</v>
-      </c>
-      <c r="H86" t="s">
-        <v>197</v>
-      </c>
       <c r="I86" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
       <c r="J86" t="s">
-        <v>232</v>
+        <v>231</v>
       </c>
     </row>
   </sheetData>

</xml_diff>